<commit_message>
[FIX] sequence in csv report
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_withholding_income_tax_text.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_withholding_income_tax_text.xlsx
@@ -21,8 +21,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -89,8 +90,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -113,13 +118,15 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[FIX] withholding tax cert report (csv)
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_withholding_income_tax_text.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_withholding_income_tax_text.xlsx
@@ -118,17 +118,19 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>